<commit_message>
Made changes as per review
</commit_message>
<xml_diff>
--- a/statistics-stroop-investigation.xlsx
+++ b/statistics-stroop-investigation.xlsx
@@ -11,12 +11,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Congruent</t>
   </si>
   <si>
     <t>Incongruent</t>
+  </si>
+  <si>
+    <t>Difference</t>
   </si>
 </sst>
 </file>
@@ -83,6 +86,9 @@
       <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
@@ -99,6 +105,14 @@
         <f t="shared" ref="K2:K25" si="2">(J2-22.02)^2</f>
         <v>7.518564</v>
       </c>
+      <c r="M2">
+        <f t="shared" ref="M2:M25" si="3">(J2-A2)</f>
+        <v>7.199</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ref="N2:N25" si="4">(M2-7.964)^2</f>
+        <v>0.585225</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
@@ -115,6 +129,14 @@
         <f t="shared" si="2"/>
         <v>10.751841</v>
       </c>
+      <c r="M3">
+        <f t="shared" si="3"/>
+        <v>1.95</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="4"/>
+        <v>36.168196</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
@@ -131,6 +153,14 @@
         <f t="shared" si="2"/>
         <v>0.649636</v>
       </c>
+      <c r="M4">
+        <f t="shared" si="3"/>
+        <v>11.65</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="4"/>
+        <v>13.586596</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
@@ -147,6 +177,14 @@
         <f t="shared" si="2"/>
         <v>40.106889</v>
       </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>7.057</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="4"/>
+        <v>0.822649</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
@@ -163,6 +201,14 @@
         <f t="shared" si="2"/>
         <v>0.613089</v>
       </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>8.134</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="4"/>
+        <v>0.0289</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1">
@@ -179,6 +225,14 @@
         <f t="shared" si="2"/>
         <v>1.304164</v>
       </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>8.64</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="4"/>
+        <v>0.456976</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1">
@@ -195,6 +249,14 @@
         <f t="shared" si="2"/>
         <v>6.512704</v>
       </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>9.88</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>3.671056</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1">
@@ -211,6 +273,14 @@
         <f t="shared" si="2"/>
         <v>21.399876</v>
       </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>8.407</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>0.196249</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1">
@@ -227,6 +297,14 @@
         <f t="shared" si="2"/>
         <v>1.582564</v>
       </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>11.361</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>11.539609</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1">
@@ -243,6 +321,14 @@
         <f t="shared" si="2"/>
         <v>18.164644</v>
       </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>11.802</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>14.730244</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1">
@@ -259,6 +345,14 @@
         <f t="shared" si="2"/>
         <v>6.270016</v>
       </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>2.196</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>33.269824</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
@@ -275,6 +369,14 @@
         <f t="shared" si="2"/>
         <v>11.397376</v>
       </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>3.346</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>21.325924</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
@@ -291,6 +393,14 @@
         <f t="shared" si="2"/>
         <v>20.3401</v>
       </c>
+      <c r="M14">
+        <f t="shared" si="3"/>
+        <v>2.437</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="4"/>
+        <v>30.547729</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
@@ -307,6 +417,14 @@
         <f t="shared" si="2"/>
         <v>2.8561</v>
       </c>
+      <c r="M15">
+        <f t="shared" si="3"/>
+        <v>3.401</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="4"/>
+        <v>20.820969</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1">
@@ -323,6 +441,14 @@
         <f t="shared" si="2"/>
         <v>175.165225</v>
       </c>
+      <c r="M16">
+        <f t="shared" si="3"/>
+        <v>17.055</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="4"/>
+        <v>82.646281</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1">
@@ -339,6 +465,14 @@
         <f t="shared" si="2"/>
         <v>0.019044</v>
       </c>
+      <c r="M17">
+        <f t="shared" si="3"/>
+        <v>10.028</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="4"/>
+        <v>4.260096</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1">
@@ -355,6 +489,14 @@
         <f t="shared" si="2"/>
         <v>9.728161</v>
       </c>
+      <c r="M18">
+        <f t="shared" si="3"/>
+        <v>6.644</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="4"/>
+        <v>1.7424</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
@@ -371,6 +513,14 @@
         <f t="shared" si="2"/>
         <v>2.531281</v>
       </c>
+      <c r="M19">
+        <f t="shared" si="3"/>
+        <v>9.79</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="4"/>
+        <v>3.334276</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1">
@@ -387,6 +537,14 @@
         <f t="shared" si="2"/>
         <v>21.114025</v>
       </c>
+      <c r="M20">
+        <f t="shared" si="3"/>
+        <v>6.081</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="4"/>
+        <v>3.545689</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1">
@@ -403,6 +561,14 @@
         <f t="shared" si="2"/>
         <v>150.503824</v>
       </c>
+      <c r="M21">
+        <f t="shared" si="3"/>
+        <v>21.919</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="4"/>
+        <v>194.742025</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1">
@@ -419,6 +585,14 @@
         <f t="shared" si="2"/>
         <v>3.511876</v>
       </c>
+      <c r="M22">
+        <f t="shared" si="3"/>
+        <v>10.95</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="4"/>
+        <v>8.916196</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1">
@@ -435,6 +609,14 @@
         <f t="shared" si="2"/>
         <v>16.4836</v>
       </c>
+      <c r="M23">
+        <f t="shared" si="3"/>
+        <v>3.727</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="4"/>
+        <v>17.952169</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1">
@@ -451,6 +633,14 @@
         <f t="shared" si="2"/>
         <v>0.001444</v>
       </c>
+      <c r="M24">
+        <f t="shared" si="3"/>
+        <v>2.348</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="4"/>
+        <v>31.539456</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1">
@@ -466,6 +656,14 @@
       <c r="K25">
         <f t="shared" si="2"/>
         <v>0.744769</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="3"/>
+        <v>5.153</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="4"/>
+        <v>7.901721</v>
       </c>
     </row>
     <row r="27">
@@ -474,16 +672,24 @@
         <v>14.051125</v>
       </c>
       <c r="B27">
-        <f>sqrt(sum(B2:B25)/24)</f>
-        <v>3.484415894</v>
+        <f>sqrt(sum(B2:B25)/23)</f>
+        <v>3.559358143</v>
       </c>
       <c r="J27">
         <f>average(J2:J25)</f>
         <v>22.01591667</v>
       </c>
       <c r="K27">
-        <f>sqrt(sum(K2:K25)/24)</f>
-        <v>4.69605691</v>
+        <f>sqrt(sum(K2:K25)/23)</f>
+        <v>4.797058936</v>
+      </c>
+      <c r="M27">
+        <f>average(M2:M25)</f>
+        <v>7.964791667</v>
+      </c>
+      <c r="N27">
+        <f>sqrt(sum(N2:N25)/23)</f>
+        <v>4.864826978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>